<commit_message>
The first version of the problem to solve is done
</commit_message>
<xml_diff>
--- a/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
+++ b/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
@@ -11,13 +11,14 @@
     <sheet name="theta" sheetId="2" r:id="rId2"/>
     <sheet name="x" sheetId="3" r:id="rId3"/>
     <sheet name="u" sheetId="4" r:id="rId4"/>
+    <sheet name="y" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Value</t>
   </si>
@@ -35,6 +36,9 @@
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -408,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.09370231628417969</v>
+        <v>8.844784736633301</v>
       </c>
     </row>
   </sheetData>
@@ -444,7 +448,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -460,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1.772631322092388e-09</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -468,7 +472,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>4.948228194339195e-09</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -476,7 +480,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>4.960662516678006e-09</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -484,7 +488,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>4.949092282335076e-09</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -492,7 +496,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>4.952604307179858e-09</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -500,7 +504,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>4.946997580557931e-09</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -508,7 +512,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>4.950494027838737e-09</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -516,7 +520,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-1</v>
+        <v>4.956516616693535e-09</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -524,7 +528,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>4.950634072583337e-09</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -532,7 +536,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>4.969736347706885e-09</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -540,7 +544,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>4.976312164647533e-09</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -548,7 +552,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>4.962573549946758e-09</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -556,7 +560,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>4.972070805337395e-09</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -564,7 +568,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>4.967706191045225e-09</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -572,7 +576,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>4.97709900485561e-09</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -580,7 +584,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-1</v>
+        <v>4.964185977511967e-09</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -588,7 +592,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>4.969130915870459e-09</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -596,7 +600,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-1</v>
+        <v>4.969231267666475e-09</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -604,7 +608,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>4.974103689085157e-09</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -612,7 +616,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>4.97583300593035e-09</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -620,7 +624,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>4.972227202281741e-09</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -628,7 +632,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-1</v>
+        <v>4.945082283844554e-09</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -636,7 +640,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-1</v>
+        <v>4.952370790346719e-09</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -644,7 +648,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.7096202417471276</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -652,7 +656,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-1</v>
+        <v>4.953787508202114e-09</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -660,7 +664,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>4.974055498773197e-09</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -668,7 +672,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>4.959312663904164e-09</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -676,7 +680,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-1</v>
+        <v>4.945758894179138e-09</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -684,7 +688,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>4.975716542812547e-09</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -692,7 +696,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>4.957877235384038e-09</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -700,7 +704,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>4.953553772236469e-09</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -708,7 +712,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-1</v>
+        <v>4.954482909114329e-09</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -716,7 +720,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>4.959750231487599e-09</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -724,7 +728,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>4.945235410836841e-09</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -732,7 +736,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>4.957419841291937e-09</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -740,7 +744,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>4.977896394624418e-09</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -748,7 +752,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-1</v>
+        <v>4.958883083713944e-09</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -756,7 +760,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>4.95220437397246e-09</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -764,7 +768,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-1</v>
+        <v>4.975426929608879e-09</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -772,7 +776,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>4.961685340894535e-09</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -780,7 +784,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>4.972426053906113e-09</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -788,7 +792,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>4.954939476616199e-09</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -796,7 +800,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>-1</v>
+        <v>4.946837169469815e-09</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -804,7 +808,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-1</v>
+        <v>4.976261115477403e-09</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -812,7 +816,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>4.953530748925933e-09</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -820,7 +824,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>4.953103371097186e-09</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -828,7 +832,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>4.982490096555154e-09</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -836,7 +840,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-1</v>
+        <v>4.976744075563257e-09</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -844,7 +848,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>4.971102114387933e-09</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -852,7 +856,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>4.95832046931804e-09</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -860,7 +864,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-1</v>
+        <v>4.965794286926654e-09</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -868,7 +872,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>4.975404219434989e-09</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -876,7 +880,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>4.968590121415123e-09</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -884,7 +888,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>4.954733323985409e-09</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -892,7 +896,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>4.974202848531104e-09</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -900,7 +904,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>4.974332393191439e-09</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -908,7 +912,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-1</v>
+        <v>4.967577691548161e-09</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -916,7 +920,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-1</v>
+        <v>4.971739365109349e-09</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -924,7 +928,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>4.983840403322138e-09</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -932,7 +936,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>4.982798761458076e-09</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -940,7 +944,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>4.967670628346606e-09</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -948,7 +952,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>4.958364528761278e-09</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -956,7 +960,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>4.97577562014994e-09</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -964,7 +968,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>4.951392862608846e-09</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -972,7 +976,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>4.975031475889907e-09</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -980,7 +984,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>4.978655134424261e-09</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -988,7 +992,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>4.960987228023804e-09</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -996,7 +1000,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>4.948026744156654e-09</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1004,7 +1008,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>4.98305041440291e-09</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1012,7 +1016,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>4.960202002507434e-09</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1020,7 +1024,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>4.962673224941002e-09</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1028,7 +1032,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>-1</v>
+        <v>4.983202791349217e-09</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1036,7 +1040,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-1</v>
+        <v>4.966981379862862e-09</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1044,7 +1048,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-1</v>
+        <v>4.945207302065851e-09</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1052,7 +1056,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>4.978756239267719e-09</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1060,7 +1064,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>-1</v>
+        <v>4.9479179985229e-09</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1068,7 +1072,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>4.972263742879051e-09</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1076,7 +1080,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-1</v>
+        <v>4.979492248091813e-09</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1084,7 +1088,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>4.972549297407462e-09</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1092,7 +1096,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>4.959600258913346e-09</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1100,7 +1104,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-1</v>
+        <v>4.952558155320024e-09</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1108,7 +1112,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>4.978853810410846e-09</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1116,7 +1120,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>-1</v>
+        <v>4.972973623091897e-09</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1124,7 +1128,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0.7090202624351183</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1132,7 +1136,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-1</v>
+        <v>4.973761053110192e-09</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1140,7 +1144,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>4.952255806839621e-09</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1148,7 +1152,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>4.956012377964787e-09</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1156,7 +1160,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>4.971334698734782e-09</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1164,7 +1168,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>4.958787140326737e-09</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1172,7 +1176,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>4.958594887967821e-09</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1180,7 +1184,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>4.960195280932114e-09</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1188,7 +1192,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-1</v>
+        <v>4.952986741801684e-09</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1196,7 +1200,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-1</v>
+        <v>4.959323383535981e-09</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1204,7 +1208,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>4.953147399041809e-09</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1212,7 +1216,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>4.980954714464776e-09</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1220,7 +1224,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>4.959789730383899e-09</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1228,7 +1232,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>4.972545453206029e-09</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1236,7 +1240,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>4.957571693200213e-09</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1244,7 +1248,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>4.951843860613708e-09</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1252,7 +1256,407 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>4.951204829839847e-09</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>4.971919570846258e-09</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>4.971861754330537e-09</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>4.977038994341173e-09</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>4.976329821517727e-09</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>0.705275042090387</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>4.967704086224255e-09</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>4.967082685316332e-09</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>4.976942670204185e-09</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>4.974422515627201e-09</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>4.965336668832455e-09</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>4.961809890484689e-09</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>4.963083416575012e-09</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>4.962852460500349e-09</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>4.980773578142742e-09</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>4.967866171156201e-09</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>4.97132854601832e-09</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>4.960108452162368e-09</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>4.948914096044145e-09</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>4.946414536775965e-09</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>4.972240546399828e-09</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>4.970310425918696e-09</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>4.975019391295412e-09</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>0.7044973475964171</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>4.958644573627087e-09</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>4.968135352761358e-09</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>4.956298359701042e-09</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>4.954819699628527e-09</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>4.945105709508022e-09</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>4.973857067433867e-09</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>4.983762455134649e-09</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>4.956030453430618e-09</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>4.965356383454422e-09</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>4.956879227153399e-09</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>4.952460455819641e-09</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>4.961343893281384e-09</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>4.953201566403645e-09</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>4.978182218768498e-09</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>4.948897846483194e-09</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>4.96629312364984e-09</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>4.978739564387384e-09</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>4.951673248469791e-09</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>4.983848779041419e-09</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>4.973835027463785e-09</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>4.980146520648424e-09</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>4.957419756648782e-09</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>4.962236388387235e-09</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>4.975357149281326e-09</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>4.977852715388436e-09</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>4.957781731431171e-09</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>4.982620110340451e-09</v>
       </c>
     </row>
   </sheetData>
@@ -1262,7 +1666,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B151"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1281,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-1.498941764782871</v>
+        <v>-1.025491719235965</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1289,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.5726947861862661</v>
+        <v>-1.758836587582003</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1297,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-1.550811675783904</v>
+        <v>-0.8176983786983505</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1305,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-0.9305770467693346</v>
+        <v>-1.693327070700814</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1313,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.843679043163776</v>
+        <v>-1.427232872661531</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1321,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-1.814585094148804</v>
+        <v>-1.85216118651203</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1329,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-1.922954657689981</v>
+        <v>-1.587089830666576</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1337,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.5181135694913732</v>
+        <v>-1.131123663615027</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1345,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.1219078963078966</v>
+        <v>-1.576478257915759</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1353,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-1.987271310292042</v>
+        <v>-0.1330505013343688</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1361,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-0.9165899286142785</v>
+        <v>0.3619614908570461</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1369,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.6053297015311827</v>
+        <v>-0.6733534270026644</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1377,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-1.0143911415835</v>
+        <v>0.04279391483330208</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1385,7 +1789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.2733636482499262</v>
+        <v>-0.2860727774270297</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1393,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-1.3455283052774</v>
+        <v>0.4211272049439394</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1401,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.01477693709021821</v>
+        <v>-0.5516255859351369</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1409,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.5260105257506142</v>
+        <v>-0.1786750279326255</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1417,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.5411032835901541</v>
+        <v>-0.1711120833397799</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1425,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-1.591969153028674</v>
+        <v>0.1958218876858941</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1433,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-0.7868332532013529</v>
+        <v>0.3259246801277786</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1441,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>-1.968384270625444</v>
+        <v>0.05457021758864933</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1449,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>0.9001166285175222</v>
+        <v>-1.997473315719062</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1457,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>0.513346181179835</v>
+        <v>-1.444917422460285</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1465,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.6314237931870936</v>
+        <v>-1.426047813317746</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1473,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.1152899485590968</v>
+        <v>-1.337645520118827</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1481,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-1.695291137561901</v>
+        <v>0.1921953822923932</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1489,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-1.035432693378833</v>
+        <v>-0.9197044060225648</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1497,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.9316775916338504</v>
+        <v>-1.946130505313933</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1505,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-1.545275374860329</v>
+        <v>0.3171648728620471</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1513,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-1.340464189401732</v>
+        <v>-1.02822103442286</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1521,7 +1925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-1.954042235633534</v>
+        <v>-1.35534069673737</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1529,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.5990780027874871</v>
+        <v>-1.285006599975327</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1537,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-1.420203990055287</v>
+        <v>-0.8866338056867975</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1545,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-1.956037335565401</v>
+        <v>-1.985852824287604</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1553,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-1.022131147549417</v>
+        <v>-1.062808922768782</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1561,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>-1.599594643178319</v>
+        <v>0.4810717520620247</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1569,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>0.6959105951737223</v>
+        <v>-0.952175413440536</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1577,7 +1981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.5567164183786244</v>
+        <v>-1.457521079667401</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1585,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.6014956447471418</v>
+        <v>0.2953801924299815</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1593,7 +1997,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-1.728658392650607</v>
+        <v>-0.7404319922607412</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1601,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-0.7162197042918477</v>
+        <v>0.06954245483389832</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1609,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-1.939207293876738</v>
+        <v>-1.250452056972108</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1617,7 +2021,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>0.4171685745220541</v>
+        <v>-1.864328467139036</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1625,7 +2029,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.9161409044301165</v>
+        <v>0.3581224081269534</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1633,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-0.5975318604422672</v>
+        <v>-1.357083759538127</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1641,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.4749832100641216</v>
+        <v>-1.389442019938829</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1649,7 +2053,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>-0.7119652838124577</v>
+        <v>0.8261234534512258</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1657,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.5376647532759558</v>
+        <v>0.3944403781887384</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1665,7 +2069,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-0.7522735195116037</v>
+        <v>-0.03015841203012881</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1673,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-1.919468737263058</v>
+        <v>-0.9947082869631791</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1681,7 +2085,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>0.779269211129102</v>
+        <v>-0.4302660392933275</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1689,7 +2093,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-1.006772838868468</v>
+        <v>0.2936718543552272</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1697,7 +2101,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-0.2308805422767</v>
+        <v>-0.2194355189449402</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1705,7 +2109,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>-0.1903381290234472</v>
+        <v>-1.266053812645353</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1713,7 +2117,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-1.757064870098519</v>
+        <v>0.2032838495769762</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1721,7 +2125,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>-1.852053916334034</v>
+        <v>0.2130320280924107</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1729,7 +2133,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0.2679248105111611</v>
+        <v>-0.2957614816815313</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1737,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.2504552797052053</v>
+        <v>0.0178354610241942</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1745,7 +2149,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-1.123094199741884</v>
+        <v>0.9274578856965077</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1753,7 +2157,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>-1.229897106833902</v>
+        <v>0.8492910865982255</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1761,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>-1.556416374064145</v>
+        <v>-0.2887541242905018</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1769,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.1519036531517088</v>
+        <v>-0.9913772039381663</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1777,7 +2181,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>-1.469438995595673</v>
+        <v>0.3216084305343259</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1785,7 +2189,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-0.6407861780659387</v>
+        <v>-1.518989985892376</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1793,7 +2197,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>-1.501035569822166</v>
+        <v>0.2656311150193504</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1801,7 +2205,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-0.674239385654559</v>
+        <v>0.5380972374482917</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1809,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>-1.784676504371353</v>
+        <v>-0.7931664771795908</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1817,7 +2221,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>-0.7106147510731258</v>
+        <v>-1.774111517520497</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1825,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-0.3819394262544256</v>
+        <v>0.8681779091439705</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1833,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-1.924533740510604</v>
+        <v>-0.8524941398257859</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1841,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-0.1170578192085918</v>
+        <v>-0.6658269435512991</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1849,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0.07044564030384048</v>
+        <v>0.8796132488258497</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1857,7 +2261,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0.7259045907542321</v>
+        <v>-0.34072747683543</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1865,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0.1631656613814441</v>
+        <v>-1.987985903767425</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1873,7 +2277,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-0.08491560641631435</v>
+        <v>0.5456950949477561</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1881,7 +2285,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0.9441813628575186</v>
+        <v>-1.782357498582343</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1889,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.8998925427380366</v>
+        <v>0.05732155456410304</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1897,7 +2301,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0.3960735713220034</v>
+        <v>0.6009978402837941</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1905,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-1.900791344099976</v>
+        <v>0.07882144237710875</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1913,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.9134335227297525</v>
+        <v>-0.8979680004924104</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1921,7 +2325,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>0.4353891053242656</v>
+        <v>-1.430727923011459</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1929,7 +2333,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-0.5542436774052342</v>
+        <v>0.5530271785698857</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1937,7 +2341,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0.7307657161329466</v>
+        <v>0.1107662425422351</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1945,7 +2349,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-1.013962511069884</v>
+        <v>-1.425308271745022</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1953,7 +2357,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>0.3001986566218831</v>
+        <v>0.1700360757237642</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1961,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-1.47021925341641</v>
+        <v>-1.453625712786084</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1969,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-0.9725428080245733</v>
+        <v>-1.169269120546788</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1977,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.7452968940582225</v>
+        <v>-0.0126405038038242</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1985,7 +2389,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.2913173740254411</v>
+        <v>-0.9594281116381027</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1993,7 +2397,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-1.789289266042518</v>
+        <v>-0.9739617500713154</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2001,7 +2405,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.1940018784881805</v>
+        <v>-0.8530020464754762</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2009,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>0.09383697386848544</v>
+        <v>-1.39827311402813</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2017,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0.6324405690822652</v>
+        <v>-0.9188941847089076</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2025,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-0.5879197764583104</v>
+        <v>-1.386108329083921</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2033,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-1.278144921319652</v>
+        <v>0.7108487030822852</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2041,7 +2445,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-0.9505999307431252</v>
+        <v>-0.8836487540671554</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2049,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>-1.660879321448428</v>
+        <v>0.07853201812980926</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2057,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-0.8014862154134974</v>
+        <v>-1.051325459232974</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2065,7 +2469,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-0.1911667477797174</v>
+        <v>-1.484826849227233</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2073,7 +2477,1625 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-1.505958078699834</v>
+        <v>-1.533234775666168</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>0.03140580681978467</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>0.02705202910173066</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>0.4166152682904976</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>0.3632893376491442</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>-1.420796830928111</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>-0.286231475378727</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>-0.3330877903531622</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>0.409372892150798</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>0.2198134769773095</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>-0.4647910620040745</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>-0.7310248159645814</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>-0.634855581722761</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>-0.6522933741681762</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>0.6972456050590643</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>-0.2740109892205576</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>-0.0131039015436536</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>-0.859563232963751</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>-1.706834688023223</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>-1.896388038219382</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>0.05557497110752241</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>-0.08979634413806226</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>0.2647219626799888</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>-1.419882546819699</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>-0.97020560221097</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>-0.2537171860121687</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>-1.147634038497515</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>-1.259516739674108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>-1.995695558241755</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>0.1772621099422778</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>0.9216093755304966</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>-1.167901623284115</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>-0.4633035952839877</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>-1.103695748025646</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>-1.438126794358277</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>-0.7662231343711063</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>-1.382006963127418</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>0.5025553164634449</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>-1.708066538519708</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>-0.3926365821366558</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>0.5444420221363693</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>-1.497750219019922</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>0.9280863137415682</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>0.1756034011420033</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>0.65014857960709</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>-1.062815323873509</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>-0.6988142052810771</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>0.2901310367029266</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>0.4777884998235513</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>-1.035442613393293</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>0.8358822391478764</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B151"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="1">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="1">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="1">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="1">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="1">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="1">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="1">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="1">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="1">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="1">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="1">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="1">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="1">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="1">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="1">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="1">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="1">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="1">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="1">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="1">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="1">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="1">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="1">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="1">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="1">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="1">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="1">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="1">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="1">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="1">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="1">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="1">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="1">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="1">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="1">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="1">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="1">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="1">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="1">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="1">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="1">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="1">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="1">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="1">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="1">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="1">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="1">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The second (and final) version of the problem to solve is done
</commit_message>
<xml_diff>
--- a/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
+++ b/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
     <sheet name="theta" sheetId="2" r:id="rId2"/>
-    <sheet name="x" sheetId="3" r:id="rId3"/>
-    <sheet name="u" sheetId="4" r:id="rId4"/>
+    <sheet name="u" sheetId="3" r:id="rId3"/>
+    <sheet name="x" sheetId="4" r:id="rId4"/>
     <sheet name="y" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29,13 +29,13 @@
     <t>theta</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>u</t>
   </si>
   <si>
     <t>i</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t>y</t>
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8.844784736633301</v>
+        <v>8.786959409713745</v>
       </c>
     </row>
   </sheetData>
@@ -455,6 +455,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -464,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.772631322092388e-09</v>
+        <v>-1.025491719235965</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -472,7 +475,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.948228194339195e-09</v>
+        <v>-1.758836587582003</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -480,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4.960662516678006e-09</v>
+        <v>-0.8176983786983505</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -488,7 +491,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>4.949092282335076e-09</v>
+        <v>-1.693327070700814</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -496,7 +499,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>4.952604307179858e-09</v>
+        <v>-1.427232872661531</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -504,7 +507,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>4.946997580557931e-09</v>
+        <v>-1.85216118651203</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -512,7 +515,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.950494027838737e-09</v>
+        <v>-1.587089830666576</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -520,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>4.956516616693535e-09</v>
+        <v>-1.131123663615027</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -528,7 +531,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>4.950634072583337e-09</v>
+        <v>-1.576478257915759</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -536,7 +539,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4.969736347706885e-09</v>
+        <v>-0.1330505013343688</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -544,7 +547,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4.976312164647533e-09</v>
+        <v>0.3619614908570461</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -552,7 +555,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>4.962573549946758e-09</v>
+        <v>-0.6733534270026644</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -560,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>4.972070805337395e-09</v>
+        <v>0.04279391483330208</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -568,7 +571,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>4.967706191045225e-09</v>
+        <v>-0.2860727774270297</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -576,7 +579,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>4.97709900485561e-09</v>
+        <v>0.4211272049439394</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -584,7 +587,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>4.964185977511967e-09</v>
+        <v>-0.5516255859351369</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -592,7 +595,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>4.969130915870459e-09</v>
+        <v>-0.1786750279326255</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -600,7 +603,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>4.969231267666475e-09</v>
+        <v>-0.1711120833397799</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -608,7 +611,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>4.974103689085157e-09</v>
+        <v>0.1958218876858941</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -616,7 +619,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>4.97583300593035e-09</v>
+        <v>0.3259246801277786</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -624,7 +627,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>4.972227202281741e-09</v>
+        <v>0.05457021758864933</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -632,7 +635,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>4.945082283844554e-09</v>
+        <v>-1.997473315719062</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -640,7 +643,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>4.952370790346719e-09</v>
+        <v>-1.444917422460285</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -648,7 +651,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>0.7096202417471276</v>
+        <v>-1.426047813317746</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -656,7 +659,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>4.953787508202114e-09</v>
+        <v>-1.337645520118827</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -664,7 +667,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>4.974055498773197e-09</v>
+        <v>0.1921953822923932</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -672,7 +675,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>4.959312663904164e-09</v>
+        <v>-0.9197044060225648</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -680,7 +683,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>4.945758894179138e-09</v>
+        <v>-1.946130505313933</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -688,7 +691,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>4.975716542812547e-09</v>
+        <v>0.3171648728620471</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -696,7 +699,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>4.957877235384038e-09</v>
+        <v>-1.02822103442286</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -704,7 +707,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>4.953553772236469e-09</v>
+        <v>-1.35534069673737</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -712,7 +715,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>4.954482909114329e-09</v>
+        <v>-1.285006599975327</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -720,7 +723,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>4.959750231487599e-09</v>
+        <v>-0.8866338056867975</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -728,7 +731,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>4.945235410836841e-09</v>
+        <v>-1.985852824287604</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -736,7 +739,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>4.957419841291937e-09</v>
+        <v>-1.062808922768782</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -744,7 +747,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>4.977896394624418e-09</v>
+        <v>0.4810717520620247</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -752,7 +755,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>4.958883083713944e-09</v>
+        <v>-0.952175413440536</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -760,7 +763,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>4.95220437397246e-09</v>
+        <v>-1.457521079667401</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -768,7 +771,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>4.975426929608879e-09</v>
+        <v>0.2953801924299815</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -776,7 +779,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>4.961685340894535e-09</v>
+        <v>-0.7404319922607412</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -784,7 +787,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>4.972426053906113e-09</v>
+        <v>0.06954245483389832</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -792,7 +795,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>4.954939476616199e-09</v>
+        <v>-1.250452056972108</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -800,7 +803,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>4.946837169469815e-09</v>
+        <v>-1.864328467139036</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -808,7 +811,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>4.976261115477403e-09</v>
+        <v>0.3581224081269534</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -816,7 +819,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>4.953530748925933e-09</v>
+        <v>-1.357083759538127</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -824,7 +827,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>4.953103371097186e-09</v>
+        <v>-1.389442019938829</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -832,7 +835,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>4.982490096555154e-09</v>
+        <v>0.8261234534512258</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -840,7 +843,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>4.976744075563257e-09</v>
+        <v>0.3944403781887384</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -848,7 +851,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>4.971102114387933e-09</v>
+        <v>-0.03015841203012881</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -856,7 +859,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>4.95832046931804e-09</v>
+        <v>-0.9947082869631791</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -864,7 +867,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>4.965794286926654e-09</v>
+        <v>-0.4302660392933275</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -872,7 +875,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>4.975404219434989e-09</v>
+        <v>0.2936718543552272</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -880,7 +883,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>4.968590121415123e-09</v>
+        <v>-0.2194355189449402</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -888,7 +891,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>4.954733323985409e-09</v>
+        <v>-1.266053812645353</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -896,7 +899,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>4.974202848531104e-09</v>
+        <v>0.2032838495769762</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -904,7 +907,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>4.974332393191439e-09</v>
+        <v>0.2130320280924107</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -912,7 +915,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>4.967577691548161e-09</v>
+        <v>-0.2957614816815313</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -920,7 +923,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>4.971739365109349e-09</v>
+        <v>0.0178354610241942</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -928,7 +931,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>4.983840403322138e-09</v>
+        <v>0.9274578856965077</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -936,7 +939,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>4.982798761458076e-09</v>
+        <v>0.8492910865982255</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -944,7 +947,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>4.967670628346606e-09</v>
+        <v>-0.2887541242905018</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -952,7 +955,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>4.958364528761278e-09</v>
+        <v>-0.9913772039381663</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -960,7 +963,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>4.97577562014994e-09</v>
+        <v>0.3216084305343259</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -968,7 +971,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>4.951392862608846e-09</v>
+        <v>-1.518989985892376</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -976,7 +979,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>4.975031475889907e-09</v>
+        <v>0.2656311150193504</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -984,7 +987,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>4.978655134424261e-09</v>
+        <v>0.5380972374482917</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -992,7 +995,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>4.960987228023804e-09</v>
+        <v>-0.7931664771795908</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1000,7 +1003,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>4.948026744156654e-09</v>
+        <v>-1.774111517520497</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1008,7 +1011,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>4.98305041440291e-09</v>
+        <v>0.8681779091439705</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1016,7 +1019,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>4.960202002507434e-09</v>
+        <v>-0.8524941398257859</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1024,7 +1027,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>4.962673224941002e-09</v>
+        <v>-0.6658269435512991</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1032,7 +1035,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>4.983202791349217e-09</v>
+        <v>0.8796132488258497</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1040,7 +1043,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>4.966981379862862e-09</v>
+        <v>-0.34072747683543</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1048,7 +1051,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>4.945207302065851e-09</v>
+        <v>-1.987985903767425</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1056,7 +1059,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>4.978756239267719e-09</v>
+        <v>0.5456950949477561</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1064,7 +1067,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>4.9479179985229e-09</v>
+        <v>-1.782357498582343</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1072,7 +1075,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>4.972263742879051e-09</v>
+        <v>0.05732155456410304</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1080,7 +1083,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>4.979492248091813e-09</v>
+        <v>0.6009978402837941</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1088,7 +1091,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>4.972549297407462e-09</v>
+        <v>0.07882144237710875</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1096,7 +1099,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>4.959600258913346e-09</v>
+        <v>-0.8979680004924104</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1104,7 +1107,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>4.952558155320024e-09</v>
+        <v>-1.430727923011459</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1112,7 +1115,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>4.978853810410846e-09</v>
+        <v>0.5530271785698857</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1120,7 +1123,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>4.972973623091897e-09</v>
+        <v>0.1107662425422351</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1128,7 +1131,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>0.7090202624351183</v>
+        <v>-1.425308271745022</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1136,7 +1139,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>4.973761053110192e-09</v>
+        <v>0.1700360757237642</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1144,7 +1147,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>4.952255806839621e-09</v>
+        <v>-1.453625712786084</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1152,7 +1155,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>4.956012377964787e-09</v>
+        <v>-1.169269120546788</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1160,7 +1163,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>4.971334698734782e-09</v>
+        <v>-0.0126405038038242</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1168,7 +1171,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>4.958787140326737e-09</v>
+        <v>-0.9594281116381027</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1176,7 +1179,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>4.958594887967821e-09</v>
+        <v>-0.9739617500713154</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1184,7 +1187,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>4.960195280932114e-09</v>
+        <v>-0.8530020464754762</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1192,7 +1195,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>4.952986741801684e-09</v>
+        <v>-1.39827311402813</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1200,7 +1203,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>4.959323383535981e-09</v>
+        <v>-0.9188941847089076</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1208,7 +1211,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>4.953147399041809e-09</v>
+        <v>-1.386108329083921</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1216,7 +1219,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>4.980954714464776e-09</v>
+        <v>0.7108487030822852</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1224,7 +1227,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>4.959789730383899e-09</v>
+        <v>-0.8836487540671554</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1232,7 +1235,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>4.972545453206029e-09</v>
+        <v>0.07853201812980926</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1240,7 +1243,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>4.957571693200213e-09</v>
+        <v>-1.051325459232974</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1248,7 +1251,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>4.951843860613708e-09</v>
+        <v>-1.484826849227233</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1256,7 +1259,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>4.951204829839847e-09</v>
+        <v>-1.533234775666168</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1264,7 +1267,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>4.971919570846258e-09</v>
+        <v>0.03140580681978467</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1272,7 +1275,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>4.971861754330537e-09</v>
+        <v>0.02705202910173066</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1280,7 +1283,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>4.977038994341173e-09</v>
+        <v>0.4166152682904976</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1288,7 +1291,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>4.976329821517727e-09</v>
+        <v>0.3632893376491442</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1296,7 +1299,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>0.705275042090387</v>
+        <v>-1.420796830928111</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1304,7 +1307,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>4.967704086224255e-09</v>
+        <v>-0.286231475378727</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1312,7 +1315,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>4.967082685316332e-09</v>
+        <v>-0.3330877903531622</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1320,7 +1323,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>4.976942670204185e-09</v>
+        <v>0.409372892150798</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1328,7 +1331,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>4.974422515627201e-09</v>
+        <v>0.2198134769773095</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1336,7 +1339,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>4.965336668832455e-09</v>
+        <v>-0.4647910620040745</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1344,7 +1347,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>4.961809890484689e-09</v>
+        <v>-0.7310248159645814</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1352,7 +1355,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>4.963083416575012e-09</v>
+        <v>-0.634855581722761</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1360,7 +1363,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>4.962852460500349e-09</v>
+        <v>-0.6522933741681762</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1368,7 +1371,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>4.980773578142742e-09</v>
+        <v>0.6972456050590643</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1376,7 +1379,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>4.967866171156201e-09</v>
+        <v>-0.2740109892205576</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -1384,7 +1387,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>4.97132854601832e-09</v>
+        <v>-0.0131039015436536</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -1392,7 +1395,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>4.960108452162368e-09</v>
+        <v>-0.859563232963751</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -1400,7 +1403,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>4.948914096044145e-09</v>
+        <v>-1.706834688023223</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -1408,7 +1411,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>4.946414536775965e-09</v>
+        <v>-1.896388038219382</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -1416,7 +1419,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>4.972240546399828e-09</v>
+        <v>0.05557497110752241</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -1424,7 +1427,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>4.970310425918696e-09</v>
+        <v>-0.08979634413806226</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -1432,7 +1435,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>4.975019391295412e-09</v>
+        <v>0.2647219626799888</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -1440,7 +1443,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0.7044973475964171</v>
+        <v>-1.419882546819699</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -1448,7 +1451,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>4.958644573627087e-09</v>
+        <v>-0.97020560221097</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -1456,7 +1459,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>4.968135352761358e-09</v>
+        <v>-0.2537171860121687</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -1464,7 +1467,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>4.956298359701042e-09</v>
+        <v>-1.147634038497515</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -1472,7 +1475,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>4.954819699628527e-09</v>
+        <v>-1.259516739674108</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -1480,7 +1483,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>4.945105709508022e-09</v>
+        <v>-1.995695558241755</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -1488,7 +1491,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>4.973857067433867e-09</v>
+        <v>0.1772621099422778</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -1496,7 +1499,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>4.983762455134649e-09</v>
+        <v>0.9216093755304966</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -1504,7 +1507,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>4.956030453430618e-09</v>
+        <v>-1.167901623284115</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -1512,7 +1515,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>4.965356383454422e-09</v>
+        <v>-0.4633035952839877</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -1520,7 +1523,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>4.956879227153399e-09</v>
+        <v>-1.103695748025646</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -1528,7 +1531,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>4.952460455819641e-09</v>
+        <v>-1.438126794358277</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -1536,7 +1539,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>4.961343893281384e-09</v>
+        <v>-0.7662231343711063</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -1544,7 +1547,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>4.953201566403645e-09</v>
+        <v>-1.382006963127418</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -1552,7 +1555,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>4.978182218768498e-09</v>
+        <v>0.5025553164634449</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -1560,7 +1563,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>4.948897846483194e-09</v>
+        <v>-1.708066538519708</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -1568,7 +1571,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>4.96629312364984e-09</v>
+        <v>-0.3926365821366558</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -1576,7 +1579,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>4.978739564387384e-09</v>
+        <v>0.5444420221363693</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -1584,7 +1587,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>4.951673248469791e-09</v>
+        <v>-1.497750219019922</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -1592,7 +1595,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>4.983848779041419e-09</v>
+        <v>0.9280863137415682</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -1600,7 +1603,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>4.973835027463785e-09</v>
+        <v>0.1756034011420033</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -1608,7 +1611,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>4.980146520648424e-09</v>
+        <v>0.65014857960709</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -1616,7 +1619,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>4.957419756648782e-09</v>
+        <v>-1.062815323873509</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -1624,7 +1627,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>4.962236388387235e-09</v>
+        <v>-0.6988142052810771</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -1632,7 +1635,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>4.975357149281326e-09</v>
+        <v>0.2901310367029266</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1640,7 +1643,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>4.977852715388436e-09</v>
+        <v>0.4777884998235513</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -1648,7 +1651,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>4.957781731431171e-09</v>
+        <v>-1.035442613393293</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -1656,7 +1659,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>4.982620110340451e-09</v>
+        <v>0.8358822391478764</v>
       </c>
     </row>
   </sheetData>
@@ -1673,11 +1676,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-1.025491719235965</v>
+        <v>-0.008362533212884391</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-1.758836587582003</v>
+        <v>-0.008196812686071159</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.8176983786983505</v>
+        <v>-0.008411903098170102</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-1.693327070700814</v>
+        <v>-0.00821109484127867</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1717,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-1.427232872661531</v>
+        <v>-0.008270119841687131</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1725,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-1.85216118651203</v>
+        <v>-0.008176634735496614</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1733,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-1.587089830666576</v>
+        <v>-0.008234458233781168</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1741,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-1.131123663615027</v>
+        <v>-0.008337811453716169</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1749,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-1.576478257915759</v>
+        <v>-0.008236806918498114</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-0.1330505013343688</v>
+        <v>-0.008583333255869059</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1765,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.3619614908570461</v>
+        <v>-0.008716426062069208</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1773,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.6733534270026644</v>
+        <v>-0.008446915936975703</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1781,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.04279391483330208</v>
+        <v>-0.008629675227311413</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1789,7 +1789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.2860727774270297</v>
+        <v>-0.008543805173801268</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1797,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.4211272049439394</v>
+        <v>-0.008732897617185429</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1805,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.5516255859351369</v>
+        <v>-0.008476897609003851</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.1786750279326255</v>
+        <v>-0.008571471226388823</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.1711120833397799</v>
+        <v>-0.00857343296194314</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1829,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.1958218876858941</v>
+        <v>-0.008670833684618752</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1837,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.3259246801277786</v>
+        <v>-0.008706457038653755</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1845,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0.05457021758864933</v>
+        <v>-0.008632814845064153</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-1.997473315719062</v>
+        <v>-0.008145599163935339</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-1.444917422460285</v>
+        <v>-0.008266143275096309</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1869,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-1.426047813317746</v>
+        <v>-0.008270385173598538</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1877,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>-1.337645520118827</v>
+        <v>0.8175742996378883</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1885,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>0.1921953822923932</v>
+        <v>-0.008669849181428581</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1893,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-0.9197044060225648</v>
+        <v>-0.008387482276836415</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>-1.946130505313933</v>
+        <v>0.9373030810195462</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>0.3171648728620471</v>
+        <v>-0.008704037447086126</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-1.02822103442286</v>
+        <v>-0.008361850619191154</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1925,7 +1925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-1.35534069673737</v>
+        <v>-0.008286355143636003</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1933,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>-1.285006599975327</v>
+        <v>0.7988499232394671</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1941,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-0.8866338056867975</v>
+        <v>-0.008395383061835274</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1949,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-1.985852824287604</v>
+        <v>-0.008148064894272739</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1957,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-1.062808922768782</v>
+        <v>-0.008353746977275145</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1965,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>0.4810717520620247</v>
+        <v>-0.008749714703404785</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1973,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-0.952175413440536</v>
+        <v>-0.008379795398783103</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1981,7 +1981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-1.457521079667401</v>
+        <v>-0.008263316394928617</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1989,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>0.2953801924299815</v>
+        <v>-0.008698038659416946</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1997,7 +1997,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.7404319922607412</v>
+        <v>-0.008430573289359557</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2005,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>0.06954245483389832</v>
+        <v>-0.008636812963755791</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2013,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-1.250452056972108</v>
+        <v>-0.008310271005368644</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2021,7 +2021,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>-1.864328467139036</v>
+        <v>-0.008174019075662906</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2029,7 +2029,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>0.3581224081269534</v>
+        <v>-0.008715361584402607</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2037,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-1.357083759538127</v>
+        <v>-0.008285961109697119</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2045,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-1.389442019938829</v>
+        <v>-0.008278639074863205</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2053,7 +2053,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>0.8261234534512258</v>
+        <v>-0.008849128051278521</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2061,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>0.3944403781887384</v>
+        <v>-0.008725452550966392</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2069,7 +2069,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-0.03015841203012881</v>
+        <v>-0.008610327860614482</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2077,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-0.9947082869631791</v>
+        <v>-0.008369741005484869</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2085,7 +2085,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-0.4302660392933275</v>
+        <v>-0.008507217725738796</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2093,7 +2093,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0.2936718543552272</v>
+        <v>-0.008697568900717786</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2101,7 +2101,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-0.2194355189449402</v>
+        <v>-0.008560928908524272</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2109,7 +2109,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>-1.266053812645353</v>
+        <v>0.7914252974303428</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0.2032838495769762</v>
+        <v>-0.008672860658859525</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2125,7 +2125,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0.2130320280924107</v>
+        <v>-0.008675511921058619</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2133,7 +2133,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-0.2957614816815313</v>
+        <v>-0.008541326809775433</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2141,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0.0178354610241942</v>
+        <v>-0.008623036426752483</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2149,7 +2149,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0.9274578856965077</v>
+        <v>-0.008879195621726994</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2157,7 +2157,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0.8492910865982255</v>
+        <v>-0.008855970246774881</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2165,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>-0.2887541242905018</v>
+        <v>-0.008543119078057172</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2173,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.9913772039381663</v>
+        <v>-0.008370527182817356</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2181,7 +2181,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0.3216084305343259</v>
+        <v>-0.008705263448752026</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2189,7 +2189,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>-1.518989985892376</v>
+        <v>0.86714867199784</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2197,7 +2197,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0.2656311150193504</v>
+        <v>-0.008689873607786199</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2205,7 +2205,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0.5380972374482917</v>
+        <v>-0.008765834918330707</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2213,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>-0.7931664771795908</v>
+        <v>-0.008417806296953882</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2221,7 +2221,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>-1.774111517520497</v>
+        <v>-0.008193491886609465</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2229,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0.8681779091439705</v>
+        <v>-0.008861568558451624</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.8524941398257859</v>
+        <v>-0.008403550227774694</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2245,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-0.6658269435512991</v>
+        <v>-0.008448757052192559</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2253,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0.8796132488258497</v>
+        <v>-0.008864972253482147</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2261,7 +2261,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-0.34072747683543</v>
+        <v>-0.008529864223059172</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-1.987985903767425</v>
+        <v>-0.008147623012643488</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0.5456950949477561</v>
+        <v>-0.9171013017100513</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>-1.782357498582343</v>
+        <v>-0.00819170752025911</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2293,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>0.05732155456410304</v>
+        <v>-0.008633550850652393</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2301,7 +2301,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0.6009978402837941</v>
+        <v>-0.9499783052364051</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2309,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>0.07882144237710875</v>
+        <v>-0.008639296745550279</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2317,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.8979680004924104</v>
+        <v>-0.008392685287222411</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2325,7 +2325,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-1.430727923011459</v>
+        <v>-0.0082693291362661</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2333,7 +2333,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0.5530271785698857</v>
+        <v>-0.008770082076552759</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2341,7 +2341,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0.1107662425422351</v>
+        <v>-0.008647860497294329</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2349,7 +2349,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-1.425308271745022</v>
+        <v>-0.008270554282885423</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2357,7 +2357,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>0.1700360757237642</v>
+        <v>-0.008663843879103536</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2365,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-1.453625712786084</v>
+        <v>-0.008264192106702862</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2373,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-1.169269120546788</v>
+        <v>-0.008328967735009872</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2381,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.0126405038038242</v>
+        <v>-0.008614960823736816</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2389,7 +2389,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.9594281116381027</v>
+        <v>-0.008378075428502904</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2397,7 +2397,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.9739617500713154</v>
+        <v>-0.008374641105153275</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2405,7 +2405,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.8530020464754762</v>
+        <v>-0.008403428461618864</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2413,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-1.39827311402813</v>
+        <v>-0.008276645011612254</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2421,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-0.9188941847089076</v>
+        <v>-0.008387698447860343</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2429,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-1.386108329083921</v>
+        <v>-0.008279389321743486</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2437,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0.7108487030822852</v>
+        <v>-0.9915140383047166</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2445,7 +2445,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-0.8836487540671554</v>
+        <v>-0.00839610327676057</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2453,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>0.07853201812980926</v>
+        <v>-0.00863921931735066</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2461,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-1.051325459232974</v>
+        <v>-0.008356428876496194</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2469,7 +2469,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-1.484826849227233</v>
+        <v>-0.008257204570087081</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2477,7 +2477,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-1.533234775666168</v>
+        <v>-0.008246406509202622</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2485,7 +2485,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>0.03140580681978467</v>
+        <v>-0.008626644016284286</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2493,7 +2493,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>0.02705202910173066</v>
+        <v>-0.00862548786519984</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2501,7 +2501,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>0.4166152682904976</v>
+        <v>-0.008731614971605572</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2509,7 +2509,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>0.3632893376491442</v>
+        <v>-0.008716795907616155</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2517,7 +2517,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>-1.420796830928111</v>
+        <v>-0.008271567698101371</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2525,7 +2525,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-0.286231475378727</v>
+        <v>-0.008543766885705512</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2533,7 +2533,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>-0.3330877903531622</v>
+        <v>-0.008531808298432414</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2541,7 +2541,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>0.409372892150798</v>
+        <v>-0.008729614994057305</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2549,7 +2549,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>0.2198134769773095</v>
+        <v>-0.008677358356134392</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2557,7 +2557,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>-0.4647910620040745</v>
+        <v>-0.00849854431954042</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>-0.7310248159645814</v>
+        <v>-0.008432856859328293</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>-0.634855581722761</v>
+        <v>-0.008456353352311079</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>-0.6522933741681762</v>
+        <v>-0.008452073197607105</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>0.6972456050590643</v>
+        <v>-0.9874424334866059</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-0.2740109892205576</v>
+        <v>-0.008546897529972477</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2605,7 +2605,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>-0.0131039015436536</v>
+        <v>-0.008614838282860977</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2613,7 +2613,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-0.859563232963751</v>
+        <v>-0.008401840831310511</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-1.706834688023223</v>
+        <v>0.9035230168581602</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-1.896388038219382</v>
+        <v>0.9311335212955568</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2637,7 +2637,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>0.05557497110752241</v>
+        <v>-0.008633084042683224</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2645,7 +2645,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>-0.08979634413806226</v>
+        <v>-0.008594640471990036</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2653,7 +2653,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>0.2647219626799888</v>
+        <v>-0.008689625359364482</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2661,7 +2661,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>-1.419882546819699</v>
+        <v>-0.008271768527650729</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2669,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>-0.97020560221097</v>
+        <v>-0.0083755278026933</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2677,7 +2677,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>-0.2537171860121687</v>
+        <v>-0.008552105413073944</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2685,7 +2685,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-1.147634038497515</v>
+        <v>-0.008333978668599598</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2693,7 +2693,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>-1.259516739674108</v>
+        <v>-0.0083081909603518</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2701,7 +2701,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>-1.995695558241755</v>
+        <v>-0.008145975579373943</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2709,7 +2709,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0.1772621099422778</v>
+        <v>-0.008665799555364</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2717,7 +2717,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>0.9216093755304966</v>
+        <v>-0.008877469037212361</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2725,7 +2725,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>-1.167901623284115</v>
+        <v>-0.008329287573658689</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2733,7 +2733,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>-0.4633035952839877</v>
+        <v>-0.008498919787189262</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2741,7 +2741,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>-1.103695748025646</v>
+        <v>-0.008344196396971431</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2749,7 +2749,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>-1.438126794358277</v>
+        <v>-0.008267664307371957</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2757,7 +2757,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>-0.7662231343711063</v>
+        <v>-0.008424327939561035</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2765,7 +2765,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>-1.382006963127418</v>
+        <v>-0.008280316331473943</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2773,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>0.5025553164634449</v>
+        <v>-0.008755774667796101</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2781,7 +2781,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>-1.708066538519708</v>
+        <v>-0.00820787179385893</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2789,7 +2789,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.3926365821366558</v>
+        <v>-0.00851670610156869</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2797,7 +2797,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0.5444420221363693</v>
+        <v>-0.008767641201340546</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2805,7 +2805,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>-1.497750219019922</v>
+        <v>-0.008254307093710615</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2813,7 +2813,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0.9280863137415682</v>
+        <v>-0.008879415177527267</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2821,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>0.1756034011420033</v>
+        <v>-0.008665351273247449</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2829,7 +2829,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0.65014857960709</v>
+        <v>-0.008797851951968945</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2837,7 +2837,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>-1.062815323873509</v>
+        <v>-0.008353736613842973</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2845,7 +2845,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>-0.6988142052810771</v>
+        <v>-0.008440698406453442</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2853,7 +2853,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0.2901310367029266</v>
+        <v>-0.008696595653236973</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2861,7 +2861,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>0.4777884998235513</v>
+        <v>-0.008748792207157647</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2869,7 +2869,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>-1.035442613393293</v>
+        <v>-0.008360155105526122</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2877,7 +2877,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0.8358822391478764</v>
+        <v>-1.020577878880851</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2911,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2919,7 +2919,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2927,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2935,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2943,7 +2943,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2951,7 +2951,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2959,7 +2959,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2967,7 +2967,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2975,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2983,7 +2983,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2991,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2999,7 +2999,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3007,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3015,7 +3015,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3023,7 +3023,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3031,7 +3031,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3311,7 +3311,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3319,7 +3319,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3327,7 +3327,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3335,7 +3335,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3343,7 +3343,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3351,7 +3351,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3359,7 +3359,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3367,7 +3367,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3375,7 +3375,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3383,7 +3383,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3391,7 +3391,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3399,7 +3399,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3407,7 +3407,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3415,7 +3415,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3431,7 +3431,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3439,7 +3439,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3447,7 +3447,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3455,7 +3455,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3463,7 +3463,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3471,7 +3471,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3479,7 +3479,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3487,7 +3487,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3495,7 +3495,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3503,7 +3503,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3511,7 +3511,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3519,7 +3519,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3527,7 +3527,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3535,7 +3535,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3543,7 +3543,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3551,7 +3551,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3559,7 +3559,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3567,7 +3567,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3575,7 +3575,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3583,7 +3583,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3591,7 +3591,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3599,7 +3599,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3607,7 +3607,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3615,7 +3615,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3623,7 +3623,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3631,7 +3631,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3639,7 +3639,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3647,7 +3647,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3655,7 +3655,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3663,7 +3663,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3671,7 +3671,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3679,7 +3679,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3687,7 +3687,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3695,7 +3695,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3703,7 +3703,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3711,7 +3711,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3719,7 +3719,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3727,7 +3727,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3735,7 +3735,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3743,7 +3743,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3751,7 +3751,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3759,7 +3759,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3767,7 +3767,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -3775,7 +3775,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -3783,7 +3783,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -3791,7 +3791,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3799,7 +3799,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -3807,7 +3807,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -3815,7 +3815,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3823,7 +3823,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3831,7 +3831,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -3839,7 +3839,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3847,7 +3847,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3855,7 +3855,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -3863,7 +3863,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -3871,7 +3871,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -3879,7 +3879,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3887,7 +3887,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -3895,7 +3895,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -3903,7 +3903,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -3911,7 +3911,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3919,7 +3919,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3927,7 +3927,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3935,7 +3935,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3943,7 +3943,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3951,7 +3951,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3959,7 +3959,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -3967,7 +3967,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3975,7 +3975,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -3983,7 +3983,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -3991,7 +3991,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -3999,7 +3999,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -4007,7 +4007,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -4015,7 +4015,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -4023,7 +4023,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4031,7 +4031,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -4039,7 +4039,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4047,7 +4047,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4055,7 +4055,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -4063,7 +4063,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -4071,7 +4071,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -4079,7 +4079,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -4087,7 +4087,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -4095,7 +4095,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The correct code is well-formatted
</commit_message>
<xml_diff>
--- a/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
+++ b/Inverse_Optimization_Related_Problem/results/Ouput_Model1/Output.xlsx
@@ -412,7 +412,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>8.786959409713745</v>
+        <v>15.58531665802002</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>-0.008362533212884391</v>
+        <v>0.8763319097879275</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1693,7 +1693,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.008196812686071159</v>
+        <v>0.04373774937504579</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1701,7 +1701,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.008411903098170102</v>
+        <v>0.03468373649165744</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>-0.00821109484127867</v>
+        <v>0.04266841321593796</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1717,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>-0.008270119841687131</v>
+        <v>0.03935354646499981</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1725,7 +1725,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>-0.008176634735496614</v>
+        <v>1.009140262103619</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1733,7 +1733,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>-0.008234458233781168</v>
+        <v>0.04118348011900557</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1741,7 +1741,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>-0.008337811453716169</v>
+        <v>0.03675866401283336</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1749,7 +1749,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>-0.008236806918498114</v>
+        <v>0.04104874882348094</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1757,7 +1757,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>-0.008583333255869059</v>
+        <v>0.0314335017432567</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1765,7 +1765,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>-0.008716426062069208</v>
+        <v>0.02971150682067697</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1773,7 +1773,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.008446915936975703</v>
+        <v>0.03388049353486607</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1781,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>-0.008629675227311413</v>
+        <v>0.0307769291871152</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1789,7 +1789,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>-0.008543805173801268</v>
+        <v>0.03205347195563703</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1797,7 +1797,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>-0.008732897617185429</v>
+        <v>0.02952935556634553</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1805,7 +1805,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>-0.008476897609003851</v>
+        <v>0.0332600788682887</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>-0.008571471226388823</v>
+        <v>0.03161328439572575</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>-0.00857343296194314</v>
+        <v>0.03158319606982835</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1829,7 +1829,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>-0.008670833684618752</v>
+        <v>0.03024760936101478</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1837,7 +1837,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>-0.008706457038653755</v>
+        <v>0.02982463242837517</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1845,7 +1845,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>-0.008632814845064153</v>
+        <v>0.03073488009708395</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>-0.008145599163935339</v>
+        <v>1.019712998852669</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1861,7 +1861,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>-0.008266143275096309</v>
+        <v>0.03953734820436428</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1869,7 +1869,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>-0.008270385173598538</v>
+        <v>0.03934137311963928</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1877,7 +1877,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>0.8175742996378883</v>
+        <v>0.03847993546200173</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1885,7 +1885,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>-0.008669849181428581</v>
+        <v>0.03025974111604739</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1893,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>-0.008387482276836415</v>
+        <v>0.0353032813806186</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1901,7 +1901,7 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>0.9373030810195462</v>
+        <v>1.016175372726841</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>-0.008704037447086126</v>
+        <v>0.02985238699994165</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1917,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>-0.008361850619191154</v>
+        <v>0.03601819190285348</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1925,7 +1925,7 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>-0.008286355143636003</v>
+        <v>0.03864539704629352</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1933,7 +1933,7 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>0.7988499232394671</v>
+        <v>0.03800628460852666</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1941,7 +1941,7 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>-0.008395383061835274</v>
+        <v>0.03509723663459581</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1949,7 +1949,7 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>-0.008148064894272739</v>
+        <v>1.018929841724191</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1957,7 +1957,7 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>-0.008353746977275145</v>
+        <v>0.03625975147309615</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1965,7 +1965,7 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>-0.008749714703404785</v>
+        <v>0.02934917141790918</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1973,7 +1973,7 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>-0.008379795398783103</v>
+        <v>0.03551075787861446</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1981,7 +1981,7 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>-0.008263316394928617</v>
+        <v>0.03967085542826821</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1989,7 +1989,7 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>-0.008698038659416946</v>
+        <v>0.02992185128470725</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1997,7 +1997,7 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>-0.008430573289359557</v>
+        <v>0.03424390906740583</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2005,7 +2005,7 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>-0.008636812963755791</v>
+        <v>0.0306817474428441</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2013,7 +2013,7 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>-0.008310271005368644</v>
+        <v>0.03770938339796523</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2021,7 +2021,7 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>-0.008174019075662906</v>
+        <v>1.010095320970243</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2029,7 +2029,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>-0.008715361584402607</v>
+        <v>0.02972347852863355</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2037,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>-0.008285961109697119</v>
+        <v>0.03866187475220857</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2045,7 +2045,7 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>-0.008278639074863205</v>
+        <v>0.03897382643452863</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2053,7 +2053,7 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>-0.008849128051278521</v>
+        <v>0.02838855691571966</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2061,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>-0.008725452550966392</v>
+        <v>0.02961097392394872</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2069,7 +2069,7 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>-0.008610327860614482</v>
+        <v>0.03104262803324215</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2077,7 +2077,7 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>-0.008369741005484869</v>
+        <v>0.03579070431973548</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2085,7 +2085,7 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>-0.008507217725738796</v>
+        <v>0.03268588703078296</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2093,7 +2093,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>-0.008697568900717786</v>
+        <v>0.02992732548652394</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2101,7 +2101,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>-0.008560928908524272</v>
+        <v>0.03177746167622392</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2109,7 +2109,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>0.7914252974303428</v>
+        <v>0.03784212831429859</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2117,7 +2117,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>-0.008672860658859525</v>
+        <v>0.03022270705672732</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2125,7 +2125,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>-0.008675511921058619</v>
+        <v>0.03019029651266226</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2133,7 +2133,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>-0.008541326809775433</v>
+        <v>0.03209441900059744</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2141,7 +2141,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>-0.008623036426752483</v>
+        <v>0.03086680935632359</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2149,7 +2149,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>-0.008879195621726994</v>
+        <v>0.02812851790354326</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2157,7 +2157,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>-0.008855970246774881</v>
+        <v>0.02832829234238862</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2165,7 +2165,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>-0.008543119078057172</v>
+        <v>0.0320647828112539</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2173,7 +2173,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>-0.008370527182817356</v>
+        <v>0.03576843225669901</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2181,7 +2181,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>-0.008705263448752026</v>
+        <v>0.02983829538716302</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2189,7 +2189,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>0.86714867199784</v>
+        <v>0.04035443593752901</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2197,7 +2197,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>-0.008689873607786199</v>
+        <v>0.03001774524176469</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2205,7 +2205,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>-0.008765834918330707</v>
+        <v>0.02918166623816583</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2213,7 +2213,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>-0.008417806296953882</v>
+        <v>0.03454149924869043</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2221,7 +2221,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>-0.008193491886609465</v>
+        <v>0.04400849107865243</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2229,7 +2229,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>-0.008861568558451624</v>
+        <v>0.02827952430562559</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2237,7 +2237,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>-0.008403550227774694</v>
+        <v>0.03488983752281195</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2245,7 +2245,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>-0.008448757052192559</v>
+        <v>0.03384071679736969</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2253,7 +2253,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>-0.008864972253482147</v>
+        <v>0.02825015273484522</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2261,7 +2261,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>-0.008529864223059172</v>
+        <v>0.03228728367407334</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>-0.008147623012643488</v>
+        <v>1.019074349557362</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>-0.9171013017100513</v>
+        <v>0.02915962735046505</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>-0.00819170752025911</v>
+        <v>0.04415846929723287</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2293,7 +2293,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>-0.008633550850652393</v>
+        <v>0.03072508887920293</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2301,7 +2301,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>-0.9499783052364051</v>
+        <v>0.02900113224157901</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2309,7 +2309,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>-0.008639296745550279</v>
+        <v>0.03064900109360261</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2317,7 +2317,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>-0.008392685287222411</v>
+        <v>0.03516727143937166</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2325,7 +2325,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>-0.0082693291362661</v>
+        <v>0.03938955251311569</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2333,7 +2333,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>-0.008770082076552759</v>
+        <v>0.02913842049286626</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2341,7 +2341,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>-0.008647860497294329</v>
+        <v>0.03053731574781805</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2349,7 +2349,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>-0.008270554282885423</v>
+        <v>0.03933378526954202</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2357,7 +2357,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>-0.008663843879103536</v>
+        <v>0.03033429025573767</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2365,7 +2365,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>-0.008264192106702862</v>
+        <v>0.0396293645455421</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2373,7 +2373,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>-0.008328967735009872</v>
+        <v>0.03705090657118943</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2381,7 +2381,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>-0.008614960823736816</v>
+        <v>0.03097799132157467</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2389,7 +2389,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>-0.008378075428502904</v>
+        <v>0.03555782499631806</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2397,7 +2397,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>-0.008374641105153275</v>
+        <v>0.0356529618729443</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2405,7 +2405,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>-0.008403428461618864</v>
+        <v>0.03489288481094</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2413,7 +2413,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>-0.008276645011612254</v>
+        <v>0.03906102735963154</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2421,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>-0.008387698447860343</v>
+        <v>0.03529817091611722</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2429,7 +2429,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>-0.008279389321743486</v>
+        <v>0.03894114387198945</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2437,7 +2437,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>-0.9915140383047166</v>
+        <v>0.02869592438405543</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2445,7 +2445,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>-0.00839610327676057</v>
+        <v>0.03507889105881718</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2453,7 +2453,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>-0.00863921931735066</v>
+        <v>0.03065002040207827</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2461,7 +2461,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>-0.008356428876496194</v>
+        <v>0.03617876503603727</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2469,7 +2469,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>-0.008257204570087081</v>
+        <v>0.03996763219164487</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2477,7 +2477,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>-0.008246406509202622</v>
+        <v>0.0405211675160703</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2485,7 +2485,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-0.008626644016284286</v>
+        <v>0.03081781060878424</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2493,7 +2493,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-0.00862548786519984</v>
+        <v>0.030833497154624</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2501,7 +2501,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>-0.008731614971605572</v>
+        <v>0.02954309312721515</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2509,7 +2509,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>-0.008716795907616155</v>
+        <v>0.0297073704817199</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2517,7 +2517,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>-0.008271567698101371</v>
+        <v>0.03928764563552023</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2525,7 +2525,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-0.008543766885705512</v>
+        <v>0.03205414094800086</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2533,7 +2533,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>-0.008531808298432414</v>
+        <v>0.03225418288526143</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2541,7 +2541,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>-0.008729614994057305</v>
+        <v>0.0295651963481484</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2549,7 +2549,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>-0.008677358356134392</v>
+        <v>0.03016783028002062</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2557,7 +2557,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>-0.00849854431954042</v>
+        <v>0.03284508073523334</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>-0.008432856859328293</v>
+        <v>0.03419195001846054</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>-0.008456353352311079</v>
+        <v>0.03367906727983902</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>-0.008452073197607105</v>
+        <v>0.03376968220804168</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>-0.9874424334866059</v>
+        <v>0.02873304872721034</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-0.008546897529972477</v>
+        <v>0.03200279060242</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2605,7 +2605,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>-0.008614838282860977</v>
+        <v>0.03097969423667087</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2613,7 +2613,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-0.008401840831310511</v>
+        <v>0.03493235250776237</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>0.9035230168581602</v>
+        <v>0.04287782246394797</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>0.9311335212955568</v>
+        <v>1.012547060783924</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2637,7 +2637,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>-0.008633084042683224</v>
+        <v>0.03073130303091414</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2645,7 +2645,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>-0.008594640471990036</v>
+        <v>0.03126679214639315</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2653,7 +2653,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>-0.008689625359364482</v>
+        <v>0.03002069488185221</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2661,7 +2661,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>-0.008271768527650729</v>
+        <v>0.03927832600249242</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2669,7 +2669,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>-0.0083755278026933</v>
+        <v>0.03562826848532147</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2677,7 +2677,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>-0.008552105413073944</v>
+        <v>0.03191824786638869</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2685,7 +2685,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-0.008333978668599598</v>
+        <v>0.03688389201551465</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2693,7 +2693,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>-0.0083081909603518</v>
+        <v>0.03778625086173282</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2701,7 +2701,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>-0.008145975579373943</v>
+        <v>1.019593833493061</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2709,7 +2709,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>-0.008665799555364</v>
+        <v>0.03030990053322799</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2717,7 +2717,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>-0.008877469037212361</v>
+        <v>0.02814327915421121</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2725,7 +2725,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>-0.008329287573658689</v>
+        <v>0.03704024986978131</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2733,7 +2733,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>-0.008498919787189262</v>
+        <v>0.03283815618271361</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2741,7 +2741,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>-0.008344196396971431</v>
+        <v>0.03655472480055769</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2749,7 +2749,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>-0.008267664307371957</v>
+        <v>0.03946629169899457</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2757,7 +2757,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>-0.008424327939561035</v>
+        <v>0.03438809215665058</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2765,7 +2765,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>-0.008280316331473943</v>
+        <v>0.03890110995547402</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2773,7 +2773,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-0.008755774667796101</v>
+        <v>0.02928562797624953</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2781,7 +2781,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>-0.00820787179385893</v>
+        <v>0.04289718703050781</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2789,7 +2789,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-0.00851670610156869</v>
+        <v>0.03251592761243068</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2797,7 +2797,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>-0.008767641201340546</v>
+        <v>0.02916325765567453</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2805,7 +2805,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>-0.008254307093710615</v>
+        <v>0.04011185500743412</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2813,7 +2813,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>-0.008879415177527267</v>
+        <v>-0.9036523360630978</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2821,7 +2821,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-0.008665351273247449</v>
+        <v>0.03031549225566159</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2829,7 +2829,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>-0.008797851951968945</v>
+        <v>0.02886302873755588</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2837,7 +2837,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>-0.008353736613842973</v>
+        <v>0.03625979683875341</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2845,7 +2845,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>-0.008440698406453442</v>
+        <v>0.0340165205695327</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2853,7 +2853,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>-0.008696595653236973</v>
+        <v>0.02993868421867408</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2861,7 +2861,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>-0.008748792207157647</v>
+        <v>0.02935892987029709</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2869,7 +2869,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>-0.008360155105526122</v>
+        <v>0.03606804604411745</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2877,7 +2877,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>-1.020577878880851</v>
+        <v>0.02836311206360224</v>
       </c>
     </row>
   </sheetData>
@@ -2903,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2911,7 +2911,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2919,7 +2919,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2927,7 +2927,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2935,7 +2935,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2943,7 +2943,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2951,7 +2951,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2959,7 +2959,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2967,7 +2967,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2975,7 +2975,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2983,7 +2983,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2991,7 +2991,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2999,7 +2999,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3007,7 +3007,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3015,7 +3015,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3023,7 +3023,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3031,7 +3031,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3311,7 +3311,7 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3319,7 +3319,7 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3327,7 +3327,7 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3335,7 +3335,7 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3343,7 +3343,7 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3351,7 +3351,7 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3359,7 +3359,7 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3367,7 +3367,7 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3375,7 +3375,7 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3383,7 +3383,7 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3391,7 +3391,7 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3399,7 +3399,7 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3407,7 +3407,7 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3415,7 +3415,7 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3423,7 +3423,7 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3431,7 +3431,7 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3439,7 +3439,7 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3447,7 +3447,7 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3455,7 +3455,7 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3463,7 +3463,7 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3471,7 +3471,7 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3479,7 +3479,7 @@
         <v>73</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3487,7 +3487,7 @@
         <v>74</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3495,7 +3495,7 @@
         <v>75</v>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3503,7 +3503,7 @@
         <v>76</v>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3511,7 +3511,7 @@
         <v>77</v>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3519,7 +3519,7 @@
         <v>78</v>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3527,7 +3527,7 @@
         <v>79</v>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3535,7 +3535,7 @@
         <v>80</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3543,7 +3543,7 @@
         <v>81</v>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3551,7 +3551,7 @@
         <v>82</v>
       </c>
       <c r="B83">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3559,7 +3559,7 @@
         <v>83</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3567,7 +3567,7 @@
         <v>84</v>
       </c>
       <c r="B85">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3575,7 +3575,7 @@
         <v>85</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3583,7 +3583,7 @@
         <v>86</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3591,7 +3591,7 @@
         <v>87</v>
       </c>
       <c r="B88">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3599,7 +3599,7 @@
         <v>88</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3607,7 +3607,7 @@
         <v>89</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3615,7 +3615,7 @@
         <v>90</v>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3623,7 +3623,7 @@
         <v>91</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3631,7 +3631,7 @@
         <v>92</v>
       </c>
       <c r="B93">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3639,7 +3639,7 @@
         <v>93</v>
       </c>
       <c r="B94">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3647,7 +3647,7 @@
         <v>94</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3655,7 +3655,7 @@
         <v>95</v>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3663,7 +3663,7 @@
         <v>96</v>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3671,7 +3671,7 @@
         <v>97</v>
       </c>
       <c r="B98">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3679,7 +3679,7 @@
         <v>98</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3687,7 +3687,7 @@
         <v>99</v>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3695,7 +3695,7 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3703,7 +3703,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3711,7 +3711,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3719,7 +3719,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3727,7 +3727,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3735,7 +3735,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3743,7 +3743,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3751,7 +3751,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3759,7 +3759,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3767,7 +3767,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -3775,7 +3775,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -3783,7 +3783,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -3791,7 +3791,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3799,7 +3799,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -3807,7 +3807,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -3815,7 +3815,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3823,7 +3823,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3831,7 +3831,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -3839,7 +3839,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3847,7 +3847,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3855,7 +3855,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -3863,7 +3863,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -3871,7 +3871,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -3879,7 +3879,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3887,7 +3887,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -3895,7 +3895,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -3903,7 +3903,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -3911,7 +3911,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3919,7 +3919,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3927,7 +3927,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3935,7 +3935,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3943,7 +3943,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3951,7 +3951,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -3959,7 +3959,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -3967,7 +3967,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -3975,7 +3975,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -3983,7 +3983,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -3991,7 +3991,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -3999,7 +3999,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -4007,7 +4007,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -4015,7 +4015,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -4023,7 +4023,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4031,7 +4031,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -4039,7 +4039,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4047,7 +4047,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4055,7 +4055,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -4063,7 +4063,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -4071,7 +4071,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -4079,7 +4079,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -4087,7 +4087,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -4095,7 +4095,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>